<commit_message>
text collection without images
</commit_message>
<xml_diff>
--- a/webscrapping school/msaces/Boletim_da_PI_-_2025-07-04.xlsx
+++ b/webscrapping school/msaces/Boletim_da_PI_-_2025-07-04.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,11 +459,6 @@
           <t>Marca</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>MarcaIM</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -487,7 +482,6 @@
           <t>Reprodução do sinal.</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -511,11 +505,6 @@
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>[IMAGE: images/747644.jpeg]</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -539,7 +528,6 @@
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -567,7 +555,6 @@
           <t>DOURO FRAGANCE</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -591,7 +578,6 @@
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -615,11 +601,6 @@
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>[IMAGE: images/747808.jpeg]</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -643,7 +624,6 @@
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -667,7 +647,6 @@
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -695,7 +674,6 @@
           <t>LA BANDIDA</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -723,11 +701,6 @@
           <t>LIMBO ATELIER</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>[IMAGE: images/747815.jpeg]</t>
-        </is>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -751,7 +724,6 @@
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -779,7 +751,6 @@
           <t>E INDUSTRIAL</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -807,7 +778,6 @@
           <t>BLACK INSPIRATION TALKS</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -835,7 +805,6 @@
           <t>JORNADA CONSCIENTE</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -859,7 +828,6 @@
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -887,11 +855,6 @@
           <t>FIDEXIS</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>[IMAGE: images/747822.jpeg]</t>
-        </is>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -915,7 +878,6 @@
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -939,7 +901,6 @@
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -963,7 +924,6 @@
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -987,7 +947,6 @@
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1011,11 +970,6 @@
         </is>
       </c>
       <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>[IMAGE: images/747831.jpeg]</t>
-        </is>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1039,7 +993,6 @@
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1067,7 +1020,6 @@
           <t>VINAGRE COM ELAS</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1095,7 +1047,6 @@
           <t>CYDALVA</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1123,7 +1074,6 @@
           <t>VALENTIA</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1151,7 +1101,6 @@
           <t>LUNTRA</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1175,7 +1124,6 @@
         </is>
       </c>
       <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1203,11 +1151,6 @@
           <t>VELAH</t>
         </is>
       </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>[IMAGE: images/747852.jpeg]</t>
-        </is>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1235,7 +1178,6 @@
           <t>FAYNA</t>
         </is>
       </c>
-      <c r="F30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1263,7 +1205,6 @@
           <t>VYNTRA</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1287,7 +1228,6 @@
         </is>
       </c>
       <c r="E32" t="inlineStr"/>
-      <c r="F32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1315,7 +1255,6 @@
           <t>LEXBUILD CONSULTING</t>
         </is>
       </c>
-      <c r="F33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1339,7 +1278,6 @@
         </is>
       </c>
       <c r="E34" t="inlineStr"/>
-      <c r="F34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1367,11 +1305,6 @@
           <t>SKILLWISE</t>
         </is>
       </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>[IMAGE: images/747858.jpeg]</t>
-        </is>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1399,7 +1332,6 @@
           <t>AQUADELTA</t>
         </is>
       </c>
-      <c r="F36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1427,7 +1359,6 @@
           <t>E INDUSTRIAL</t>
         </is>
       </c>
-      <c r="F37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1455,7 +1386,6 @@
           <t>SIMULADOR SU</t>
         </is>
       </c>
-      <c r="F38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1479,7 +1409,6 @@
         </is>
       </c>
       <c r="E39" t="inlineStr"/>
-      <c r="F39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1507,11 +1436,6 @@
           <t>TRANCAS</t>
         </is>
       </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>[IMAGE: images/747864.jpeg]</t>
-        </is>
-      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1539,7 +1463,6 @@
           <t>MAGMASA</t>
         </is>
       </c>
-      <c r="F41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1563,7 +1486,6 @@
         </is>
       </c>
       <c r="E42" t="inlineStr"/>
-      <c r="F42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1587,7 +1509,6 @@
         </is>
       </c>
       <c r="E43" t="inlineStr"/>
-      <c r="F43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1615,7 +1536,6 @@
           <t>POS1000</t>
         </is>
       </c>
-      <c r="F44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1643,7 +1563,6 @@
           <t>CARVALHAIS VILLAGE</t>
         </is>
       </c>
-      <c r="F45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1667,11 +1586,6 @@
         </is>
       </c>
       <c r="E46" t="inlineStr"/>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>[IMAGE: images/747871.jpeg]</t>
-        </is>
-      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1699,7 +1613,6 @@
           <t>NATHA COFFEE</t>
         </is>
       </c>
-      <c r="F47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1723,7 +1636,6 @@
         </is>
       </c>
       <c r="E48" t="inlineStr"/>
-      <c r="F48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1747,7 +1659,6 @@
         </is>
       </c>
       <c r="E49" t="inlineStr"/>
-      <c r="F49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1771,7 +1682,6 @@
         </is>
       </c>
       <c r="E50" t="inlineStr"/>
-      <c r="F50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1795,7 +1705,6 @@
         </is>
       </c>
       <c r="E51" t="inlineStr"/>
-      <c r="F51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1819,11 +1728,6 @@
         </is>
       </c>
       <c r="E52" t="inlineStr"/>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>[IMAGE: images/747920.jpeg]</t>
-        </is>
-      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1851,7 +1755,6 @@
           <t>E INDUSTRIAL</t>
         </is>
       </c>
-      <c r="F53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1879,7 +1782,6 @@
           <t>BILIBOT</t>
         </is>
       </c>
-      <c r="F54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1899,11 +1801,6 @@
       </c>
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="inlineStr"/>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>[IMAGE: images/58224.jpeg]</t>
-        </is>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>